<commit_message>
Created second Map, rewrote the terrible spawner logic (still bad), rend bar works now
</commit_message>
<xml_diff>
--- a/Dps.xlsx
+++ b/Dps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Godot\td-roguelike\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231343CC-68ED-41A9-AD32-1084AD648535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B00A0CEA-56B2-46F7-B5A6-9D74722E36C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{E83D7D76-09A5-4954-9C72-0A42614B2D2C}"/>
+    <workbookView xWindow="57480" yWindow="7125" windowWidth="29040" windowHeight="15720" xr2:uid="{E83D7D76-09A5-4954-9C72-0A42614B2D2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -454,7 +454,7 @@
   <dimension ref="A1:T26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
Added roadblocks, rescripted enemy pathing again, now reacts dynamically to the map changing
</commit_message>
<xml_diff>
--- a/Dps.xlsx
+++ b/Dps.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Godot\td-roguelike\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B00A0CEA-56B2-46F7-B5A6-9D74722E36C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF33314-DB2F-4B45-8D14-6FE6B70E5136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="7125" windowWidth="29040" windowHeight="15720" xr2:uid="{E83D7D76-09A5-4954-9C72-0A42614B2D2C}"/>
+    <workbookView xWindow="57480" yWindow="7125" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{E83D7D76-09A5-4954-9C72-0A42614B2D2C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ranged_unit" sheetId="1" r:id="rId1"/>
+    <sheet name="Ground Unit" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="8">
   <si>
     <t>Damage</t>
   </si>
@@ -54,6 +56,12 @@
   </si>
   <si>
     <t>Increase armour by 50% -&gt; dps increments by 333</t>
+  </si>
+  <si>
+    <t>Mace</t>
+  </si>
+  <si>
+    <t>Ground</t>
   </si>
 </sst>
 </file>
@@ -453,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64BD213E-97E0-4528-BD41-7D31F7328D85}">
   <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="A2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1192,4 +1200,207 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7972D139-6AED-4AE2-AC0D-764654C64CA7}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A2" s="3">
+        <v>230</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C2" s="3">
+        <v>25</v>
+      </c>
+      <c r="D2" s="3">
+        <f>A2 / (1 + (C2 / 100))</f>
+        <v>184</v>
+      </c>
+      <c r="E2" s="3">
+        <f>D2 * (1 / B2) * 10</f>
+        <v>1672.7272727272727</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A3" s="3">
+        <v>140</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="C3" s="3">
+        <v>25</v>
+      </c>
+      <c r="D3" s="3">
+        <f>A3 / (1 + (C3 / 100))</f>
+        <v>112</v>
+      </c>
+      <c r="E3" s="3">
+        <f t="shared" ref="E3" si="0">D3 * (1 / B3) * 10</f>
+        <v>1600</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9847FEE-576C-476D-99C5-EB5231A3AF0E}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <f>A2 / (1 + (C2 / 100))</f>
+        <v>1</v>
+      </c>
+      <c r="E2" s="3">
+        <f>D2 * B2 * 10</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <f>A3 / (1 + (C3 / 100))</f>
+        <v>2</v>
+      </c>
+      <c r="E3" s="3">
+        <f>D3 * B3 * 10</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A4" s="3">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <f>A4 / (1 + (C4 / 100))</f>
+        <v>6</v>
+      </c>
+      <c r="E4" s="3">
+        <f>D4 * B4 * 10</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A5" s="3">
+        <v>18</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
+        <f>A5 / (1 + (C5 / 100))</f>
+        <v>18</v>
+      </c>
+      <c r="E5" s="3">
+        <f>D5 * B5 * 10</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A6" s="3">
+        <v>12</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
+        <f>A6 / (1 + (C6 / 100))</f>
+        <v>12</v>
+      </c>
+      <c r="E6" s="3">
+        <f>D6 * B6 * 10</f>
+        <v>240</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>